<commit_message>
updated csv files - ks hyperparams
</commit_message>
<xml_diff>
--- a/kss_ks/ks_hyperparameters_and_other_details.xlsx
+++ b/kss_ks/ks_hyperparameters_and_other_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanka\Documents\github\ST_GNN_HAR_DEML\kss_ks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04827E-8284-4A24-B44C-8885D0620EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF215DCC-4BD3-402D-91A0-F97DB417C220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BODY_25" sheetId="3" r:id="rId1"/>
@@ -437,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +516,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -553,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -568,6 +574,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -601,7 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A2EB41-E4E0-4D2E-B4C9-31A38036C9D1}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +960,7 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -982,7 +989,7 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1006,7 +1013,7 @@
       <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1080,17 +1087,17 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1111,10 +1118,10 @@
       <c r="H14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="16" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1134,14 +1141,14 @@
       <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="13"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -1157,14 +1164,14 @@
       <c r="H17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="I17" s="15"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -1180,16 +1187,16 @@
       <c r="H19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="I19" s="15"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1205,12 +1212,12 @@
       <c r="I22" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1220,9 +1227,9 @@
       <c r="I24" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:13" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:14" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
@@ -1238,15 +1245,15 @@
       <c r="I25" t="s">
         <v>42</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="K25" s="15"/>
-      <c r="M25" s="19" t="s">
+      <c r="K25" s="17"/>
+      <c r="M25" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -1256,13 +1263,13 @@
       <c r="H26" t="s">
         <v>60</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="M26" s="19" t="s">
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="M26" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
@@ -1275,20 +1282,20 @@
       <c r="I27" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
       <c r="L27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M27" s="19" t="s">
+      <c r="M27" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+    </row>
+    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
@@ -1307,20 +1314,20 @@
       <c r="I29" t="s">
         <v>65</v>
       </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
       <c r="L29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M29" s="19" t="s">
+      <c r="M29" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+    </row>
+    <row r="31" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
@@ -1342,18 +1349,19 @@
       <c r="I31" t="s">
         <v>68</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
       <c r="L31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M31" s="19" t="s">
+      <c r="M31" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
+      <c r="N31" s="9"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
     </row>
     <row r="33" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1362,6 +1370,7 @@
       <c r="B33">
         <v>50</v>
       </c>
+      <c r="C33" s="1"/>
       <c r="D33">
         <v>1E-3</v>
       </c>
@@ -1377,15 +1386,15 @@
       <c r="I33" t="s">
         <v>71</v>
       </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="M33" s="19" t="s">
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="M33" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1409,18 +1418,18 @@
       <c r="I35" t="s">
         <v>71</v>
       </c>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
       <c r="L35" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M35" s="19" t="s">
+      <c r="M35" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
     </row>
     <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1441,12 +1450,12 @@
       <c r="I37" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
     </row>
     <row r="39" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1470,9 +1479,9 @@
       <c r="I39" t="s">
         <v>71</v>
       </c>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="M39" s="19" t="s">
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="M39" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1498,15 +1507,15 @@
       <c r="I41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J41" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="M41" s="19" t="s">
+      <c r="M41" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J42" s="8"/>
+      <c r="J42" s="10"/>
     </row>
     <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1530,8 +1539,8 @@
       <c r="I43" t="s">
         <v>81</v>
       </c>
-      <c r="J43" s="8"/>
-      <c r="M43" s="19" t="s">
+      <c r="J43" s="10"/>
+      <c r="M43" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1557,15 +1566,15 @@
       <c r="I46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="J46" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="M46" s="19" t="s">
+      <c r="M46" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J47" s="9"/>
+      <c r="J47" s="11"/>
     </row>
     <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -1589,8 +1598,8 @@
       <c r="I48" t="s">
         <v>81</v>
       </c>
-      <c r="J48" s="9"/>
-      <c r="M48" s="19" t="s">
+      <c r="J48" s="11"/>
+      <c r="M48" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1612,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595B1B92-5722-4419-B1AD-6E68DC0AEB96}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView topLeftCell="A7" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,13 +1704,13 @@
       <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1724,15 +1733,15 @@
       <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="19" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1759,15 +1768,15 @@
       <c r="K6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="19" t="s">
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1794,15 +1803,15 @@
       <c r="K8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="19" t="s">
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1826,15 +1835,15 @@
       <c r="K10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="19" t="s">
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1858,14 +1867,14 @@
       <c r="K12" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="19" t="s">
+      <c r="L12" s="18"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M13" s="17"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1912,10 +1921,10 @@
       <c r="L16" t="s">
         <v>107</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="M16" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="N16" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1941,8 +1950,8 @@
       <c r="L17" t="s">
         <v>107</v>
       </c>
-      <c r="M17" s="18"/>
-      <c r="N17" s="19" t="s">
+      <c r="M17" s="20"/>
+      <c r="N17" s="8" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>